<commit_message>
feat: try evaluate uni test using ragas
</commit_message>
<xml_diff>
--- a/test/adaptive/configs/list_qa.xlsx
+++ b/test/adaptive/configs/list_qa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Features\Documents\PMB-UNDIKSHA\va-pmb-undiksha\test\adaptive\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F20FCB-1294-4511-A94A-FFAD26DAEB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A6B8E1-EB9C-4187-915B-4884141E2497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A7FD8239-2D96-4688-A048-ADBE3AAB3502}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A7FD8239-2D96-4688-A048-ADBE3AAB3502}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="2" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>FE.pdf</t>
   </si>
   <si>
-    <t>Siapa nama Wakil Dekan I Fakultas Ekonomi (FE)?</t>
-  </si>
-  <si>
     <t>FHIS.pdf</t>
   </si>
   <si>
@@ -147,21 +144,9 @@
     <t>Dimana saya bisa melihat KTM?</t>
   </si>
   <si>
-    <t>Presiden</t>
-  </si>
-  <si>
     <t>Out Of Context</t>
   </si>
   <si>
-    <t>Siapa presiden indonesia sekarang?</t>
-  </si>
-  <si>
-    <t>Siapa nama Dekan Fakultas Ilmu Pendidikan (FIP)?</t>
-  </si>
-  <si>
-    <t>Kapan Fakultas Ilmu Pendidikan (FIP) Universitas Pendidikan Ganesha mulai berdiri dan apa jurusan awalnya?</t>
-  </si>
-  <si>
     <t>Kapan Fakultas Kedokteran (FK) Universitas Pendidikan Ganesha didirikan?</t>
   </si>
   <si>
@@ -247,9 +232,6 @@
   </si>
   <si>
     <t>Apa prinsip SNPMB?</t>
-  </si>
-  <si>
-    <t>Kapan jadwal pendaftaran untuk Seleksi Mandiri (SMBJM)?</t>
   </si>
   <si>
     <t>Kapan jadwal SNBP?</t>
@@ -296,10 +278,6 @@
   </si>
   <si>
     <t>Salam Harmoni🙏
-Nama Wakil Dekan I Fakultas Ekonomi (FE) Universitas Pendidikan Ganesha adalah Dr. Dra. Ni Made Suci, M.Si.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
 Nama dekan Fakultas Ilmu Pendidikan (FIP) Universitas Pendidikan Ganesha adalah Prof. Dr. I Wayan Widiana, S.Pd., M.Pd.</t>
   </si>
   <si>
@@ -340,10 +318,6 @@
 1. Lulusan SMA/SMK/MA/Sederajat tahun 2023, 2024, dan 2025.
 2. Lulusan Paket C tahun 2023, 2024, dan 2025 dengan umur maksimal 25 tahun (per 1 Juli 2025).
 Pastikan untuk memenuhi kriteria tersebut jika Anda berencana untuk mengikuti UTBK.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Jadwal pendaftaran untuk Seleksi Mahasiswa Baru Jalur Mandiri (SMBJM) Universitas Pendidikan Ganesha Tahun 2025 akan diinformasikan segera. Untuk informasi lebih lanjut, silakan pantau situs resmi Undiksha atau media sosial resmi kami.</t>
   </si>
   <si>
     <t>Salam Harmoni🙏
@@ -368,10 +342,6 @@
   </si>
   <si>
     <t>Salam Harmoni🙏
-Pertanyaan tersebut tidak relevan dengan konteks kampus Universitas Pendidikan Ganesha.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
 Program Adik Papua ialah program keberpihakan bagi putra-putri asli Papua di Provinsi Papua dan Provinsi Papua Barat dengan memberi kesempatan belajar di perguruan tinggi negeri yang diselenggarakan oleh Kemdikbud melalui mekanisme seleksi khusus siswa SMA sederajat, berdasarkan penjaringan prestasi akademik. Daerah yang menjadi sasaran pelaksanaan di Provinsi Papua dan Provinsi Papua Barat, meliputi; Kabupaten/Kota yang memiliki SMA sederajat dan memenuhi syarat sebagai peserta program ADik papua, sebagaimana diatur oleh Undang-Undang. Website resmi: https://adik.kemdikbud.go.id</t>
   </si>
   <si>
@@ -383,10 +353,6 @@
 1. Calon mahasiswa yang BELUM mendapatkan tempat kuliah.
 2. Calon mahasiswa yang TIDAK lolos pada seleksi SNMPTN atau SBMPTN.
 3. Calon mahasiswa yang SUDAH lolos pada seleksi SNMPTN atau SBMPTN tetapi hendak membatalkan pilihannya dan ingin memilih kampus atau Program Studi yang lain.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-NISN adalah Nomor Induk Siswa Nasional. Informasi NISN bisa dicari pada laman berikut http://nisn.data.kemdikbud.go.id/page/data</t>
   </si>
   <si>
     <t>Fasilitas apa saja yang dimiliki undiksha?</t>
@@ -420,10 +386,6 @@
   </si>
   <si>
     <t>Sebutkan program doktoral yang ditawarkan oleh Fakultas Pascasarjana Universitas Pendidikan Ganesha.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Informasi lebih lanjut mengenai prosedur pembayaran Uang Kuliah Tunggal (UKT) mahasiswa baru Universitas Pendidikan Ganesha dengan layanan BRI Virtual Account (BRIVA) dapat ditemukan di situs resmi Undiksha melalui tautan berikut:https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva/.</t>
   </si>
   <si>
     <t>Salam Harmoni🙏
@@ -515,9 +477,6 @@
 Contoh penulisan pesan yang benar adalah:
 - Cek Kelulusan Nomor Pendaftaran 1234567890 Tanggal Lahir 2001-01-31
 Silakan kirimkan informasi tersebut jika Anda memerlukan bantuan lebih lanjut.</t>
-  </si>
-  <si>
-    <t>Gimana cara lihat KTM? NIM saya 2115101014</t>
   </si>
   <si>
     <t>Salam Harmoni🙏
@@ -553,9 +512,6 @@
     <t>Apa jenis-jenis beasiswa bagi mahasiswa undiksha?</t>
   </si>
   <si>
-    <t>Dimana bisa melihat data NISN?</t>
-  </si>
-  <si>
     <t>Salam Harmoni🙏
 Anda dapat melihat informasi daya tampung mahasiswa baru Universitas Pendidikan Ganesha tahun akademik 2024/2025 dengan mengunjungi tautan berikut: https://undiksha.ac.id/pmb/tahun2024/daya-tampung.</t>
   </si>
@@ -572,13 +528,6 @@
   <si>
     <t>Salam Harmoni🙏
 Ya, Fakultas Hukum dan Ilmu Sosial (FHIS) Universitas Pendidikan Ganesha memiliki video profil. Anda dapat menontonnya melalui tautan berikut: https://youtu.be/xrruGWs5HNk. Video ini memberikan informasi mengenai program studi, kegiatan, dan keunggulan yang ditawarkan oleh FHIS</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Berikut informasi mengenai Kartu Tanda Mahasiswa (KTM) Anda. 
-- NIM: 2115101014
-- Anda dapat mengunduh KTM Anda melalui tautan berikut: [Download KTM](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=NVNnV1dvQ2ZLRk10bFhQSFdpazBDTkZQaUpQQjl4SUg5YTJGOExSK3hzOVdFdWhGQjdGV1VtZWVRRWNCQXhHNGlzOVI0blUxM2F4cXBaQUFUWGVwcUdtcjZmM0lyNW1ibEtSRG9pbTBxOGpBamp5R3BlSU1yZ2dZd053aE1VeTFkQWJINEZWOUx5NFdTR1pjUnA3SFdqejBvOU42QmFURVlxeEEzY21BR0JVRUdmNHI2TmJ2UFlnYktNNXE3dmVLWWFOM0tDL0p1UnFGMnZoYzV5U1RJZmlSNjlyTkdGRG1tWFc1L3B4QUZHdGJ2SHVHSTJhWjdPQXBYZlNWMzVTSERSWXJ4T3ZEMmdUak9hdm5UT1hsT0M0Yi9pbG96ZUNGeEtmRDZKZlB2VitnUWNkZnpvcmxtMkFtcWJmcEo2TTYvRFpFVjB4MkNwdFdJVUVqVGtsNVdveFVPazhNQWtVeTlnNndPWkRpTEcyblRISDJWMm41T2pLQlFidjBpMDJJVS9DQnRHQXVzbWFVQkhrMm5tSHVHZnpRN3NDUlU4ZFlaRm1jWTV2eDFONTFjMTg0NEc1Z0tMdm9GS2c9).
-Silakan klik tautan tersebut untuk mengakses KTM Anda.</t>
   </si>
   <si>
     <t>Salam Harmoni🙏
@@ -590,21 +539,6 @@
 - Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
 - Status Kelulusan: Lulus
 Selamat bergabung menjadi bagian dari Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!</t>
-  </si>
-  <si>
-    <t>Bagaimana Prosedur Pembayaran UKT Mahasiswa Baru Undiksha dengan Layanan BRI Virtual Account (BRIVA)?</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-BRI Virtual Account (BRIVA) adalah serangkaian Kode Unik yang terdiri dari beberapa digit sebagai Nomor Rekening Tujuan Pembayaran Premi Pemegang Polis. Layanan BRI Virtual Account (BRIVA) ini memberikan kemudahan dalam pemanfaatan sistem layanan jasa perbankan yang cepat, nyaman, modern, dan terpercaya. BRIVA merupakan virtual account perbankan dengan sistem real time online, sehingga seluruh pembayaran melalui BRI Virtual Account dapat langsung tercatat secara real time online di sistem verifikasi Universitas Pendidikan Ganesha.
-Informasi Prosedur Pembayaran UKT Mahasiswa Baru Undiksha dengan Layanan BRI Virtual Account (BRIVA) kunjungi: https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva/</t>
-  </si>
-  <si>
-    <t>Video profil FE</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Anda dapat menonton video profil Fakultas Ekonomi Universitas Pendidikan Ganesha melalui tautan berikut: https://youtu.be/yPoTT-M-saM. Video ini memberikan informasi mengenai program studi, visi, misi, serta berbagai kegiatan yang ada di Fakultas Ekonomi.</t>
   </si>
   <si>
     <t>Salam Harmoni🙏
@@ -619,6 +553,71 @@
 8. Beasiswa Rektor Undiksha
 9. Beasiswa dari berbagai Pemda
 Beasiswa ini ditujukan untuk mahasiswa berprestasi maupun mahasiswa kurang mampu, dan pengelolaan, pendaftaran, serta seleksi beasiswa diselenggarakan secara online maupun offline.</t>
+  </si>
+  <si>
+    <t>Salam Harmoni🙏
+Estimasi biaya kuliah adalah perkiraan biaya yang harus ditanggung oleh calon mahasiswa per semester jika mengikuti perkuliahan di Universitas Pendidikan Ganesha (Undiksha). Biaya ini mencakup berbagai komponen, seperti biaya pendidikan, biaya administrasi, dan biaya lainnya yang mungkin diperlukan selama proses perkuliahan. Estimasi ini penting untuk membantu calon mahasiswa merencanakan keuangan mereka selama menempuh pendidikan di Undiksha.</t>
+  </si>
+  <si>
+    <t>Apa itu Estimasi Biaya Kuliah?</t>
+  </si>
+  <si>
+    <t>Visi Fakultas Ekonomi</t>
+  </si>
+  <si>
+    <t>Salam Harmoni🙏
+Visi Fakultas Ekonomi (FE) Universitas Pendidikan Ganesha adalah "Menjadi Fakultas Unggul Berjiwa Wirausaha Berlandaskan Falsafah Tri Hita Karana di Asia Tahun 2045."</t>
+  </si>
+  <si>
+    <t>Kapan jadwal pendaftaran SMBJM?</t>
+  </si>
+  <si>
+    <t>Bagaimana cara ngoding?</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>Siapa nama Wakil Dekan I FE?</t>
+  </si>
+  <si>
+    <t>Salam Harmoni🙏
+Wakil Dekan I Fakultas Ekonomi (FE) Universitas Pendidikan Ganesha adalah Dr. Dra. Ni Made Suci, M.Si.</t>
+  </si>
+  <si>
+    <t>Siapa nama Dekan FIP?</t>
+  </si>
+  <si>
+    <t>Kapan FIP mulai berdiri dan apa jurusan awalnya?</t>
+  </si>
+  <si>
+    <t>Link informasi cara pembayaran UKT Mahasiswa Baru Undiksha dengan Layanan BRI Virtual Account (BRIVA)</t>
+  </si>
+  <si>
+    <t>Salam Harmoni🙏
+Informasi lebih lanjut mengenai prosedur pembayaran Uang Kuliah Tunggal (UKT) mahasiswa baru Universitas Pendidikan Ganesha dengan layanan BRI Virtual Account (BRIVA) dapat ditemukan di situs resmi Undiksha melalui tautan berikut: https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva/.</t>
+  </si>
+  <si>
+    <t>Salam Harmoni🙏
+Anda dapat mengakses informasi mengenai tata cara pembayaran Uang Kuliah Tunggal (UKT) mahasiswa baru Universitas Pendidikan Ganesha dengan layanan BRI Virtual Account (BRIVA) melalui link berikut: https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva</t>
+  </si>
+  <si>
+    <t>Saya ingin lihat KTM, NIM saya 2115101014.</t>
+  </si>
+  <si>
+    <t>Salam Harmoni🙏
+Berikut informasi Kartu Tanda Mahasiswa (KTM) Anda. 
+- NIM: 2115101014
+- Anda dapat mengunduh KTM Anda melalui tautan berikut: https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=NVNnV1dvQ2ZLRk10bFhQSFdpazBDTkZQaUpQQjl4SUg5YTJGOExSK3hzOVdFdWhGQjdGV1VtZWVRRWNCQXhHNGlzOVI0blUxM2F4cXBaQUFUWGVwcUdtcjZmM0lyNW1ibEtSRG9pbTBxOGpBamp5R3BlSU1yZ2dZd053aE1VeTFkQWJINEZWOUx5NFdTR1pjUnA3SFdqejBvOU42QmFURVlxeEEzY21BR0JVRUdmNHI2TmJ2UFlnYktNNXE3dmVLWWFOM0tDL0p1UnFGMnZoYzV5U1RJZmlSNjlyTkdGRG1tWFc1L3B4QUZHdGJ2SHVHSTJhWjdPQXBYZlNWMzVTSERSWXJ4T3ZEMmdUak9hdm5UT1hsT0M0Yi9pbG96ZUNGeEtmRDZKZlB2VitnUWNkZnpvcmxtMkFtcWJmcEo2TTYvRFpFVjB4MkNwdFdJVUVqVGtsNVdveFVPazhNQWtVeTlnNndPWkRpTEcyblRISDJWMm41T2pLQlFidjBpMDJJVS9DQnRHQXVzbWFVQkhrMm5tSHVHZnpRN3NDUlU4ZFlaRm1jWTV2eDFONTFjMTg0NEc1Z0tMdm9GS2c9.
+Silakan klik tautan tersebut untuk mengakses KTM Anda.</t>
+  </si>
+  <si>
+    <t>Salam Harmoni🙏
+Maaf, saya tidak memiliki informasi tentang cara ngoding. Namun, jika Anda memiliki pertanyaan terkait Universitas Pendidikan Ganesha, saya siap membantu.</t>
+  </si>
+  <si>
+    <t>Salam Harmoni🙏
+Jadwal pendaftaran seleksi mahasiswa baru jalur mandiri (SMBJM) Universitas Pendidikan Ganesha untuk tahun 2025 akan diinformasikan segera. Untuk informasi lebih lanjut, Anda dapat mengunjungi situs resmi Undiksha atau mengikuti pengumuman resmi dari pihak universitas.</t>
   </si>
 </sst>
 </file>
@@ -1156,13 +1155,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C236C3-56F3-4E8C-AE3B-EC9AC92EE935}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="C48" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="100.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -1177,16 +1176,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="300" x14ac:dyDescent="0.2">
@@ -1200,10 +1199,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="195" x14ac:dyDescent="0.2">
@@ -1220,7 +1219,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.2">
@@ -1234,10 +1233,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.2">
@@ -1254,7 +1253,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.2">
@@ -1271,10 +1270,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="150" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1285,10 +1284,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="360" x14ac:dyDescent="0.2">
@@ -1302,10 +1301,10 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="135" x14ac:dyDescent="0.2">
@@ -1322,7 +1321,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.2">
@@ -1339,7 +1338,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
@@ -1356,7 +1355,7 @@
         <v>13</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.2">
@@ -1370,13 +1369,13 @@
         <v>3</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="105" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1387,10 +1386,10 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.2">
@@ -1398,16 +1397,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="120" x14ac:dyDescent="0.2">
@@ -1415,16 +1414,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.2">
@@ -1432,16 +1431,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.2">
@@ -1449,16 +1448,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.2">
@@ -1466,16 +1465,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="90" x14ac:dyDescent="0.2">
@@ -1483,16 +1482,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="105" x14ac:dyDescent="0.2">
@@ -1500,16 +1499,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.2">
@@ -1517,16 +1516,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.2">
@@ -1534,16 +1533,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="105" x14ac:dyDescent="0.2">
@@ -1551,16 +1550,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.2">
@@ -1568,16 +1567,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="75" x14ac:dyDescent="0.2">
@@ -1585,16 +1584,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="75" x14ac:dyDescent="0.2">
@@ -1602,16 +1601,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="255" x14ac:dyDescent="0.2">
@@ -1619,16 +1618,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.2">
@@ -1636,16 +1635,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="150" x14ac:dyDescent="0.2">
@@ -1653,50 +1652,50 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="255" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="120" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="135" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:5" ht="120" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="180" x14ac:dyDescent="0.2">
@@ -1704,16 +1703,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="E32" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="255" x14ac:dyDescent="0.2">
@@ -1721,16 +1720,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="105" x14ac:dyDescent="0.2">
@@ -1738,16 +1737,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="225" x14ac:dyDescent="0.2">
@@ -1755,16 +1754,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="E35" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="195" x14ac:dyDescent="0.2">
@@ -1772,16 +1771,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="195" x14ac:dyDescent="0.2">
@@ -1789,16 +1788,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="75" x14ac:dyDescent="0.2">
@@ -1806,16 +1805,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="360" x14ac:dyDescent="0.2">
@@ -1823,16 +1822,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.2">
@@ -1840,16 +1839,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="255" x14ac:dyDescent="0.2">
@@ -1857,16 +1856,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.2">
@@ -1874,16 +1873,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="90" x14ac:dyDescent="0.2">
@@ -1891,16 +1890,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="135" x14ac:dyDescent="0.2">
@@ -1908,16 +1907,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="75" x14ac:dyDescent="0.2">
@@ -1925,16 +1924,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.2">
@@ -1942,16 +1941,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="210" x14ac:dyDescent="0.2">
@@ -1959,16 +1958,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="E47" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="300" x14ac:dyDescent="0.2">
@@ -1976,33 +1975,33 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="E48" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="375" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="345" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D49" s="3" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="225" x14ac:dyDescent="0.2">
@@ -2010,36 +2009,35 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="E50" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.2"/>
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>